<commit_message>
Agregando funciones nuevas a la automatización
</commit_message>
<xml_diff>
--- a/Data/FilterData.xlsx
+++ b/Data/FilterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BDGSA\Documents\UiPath\ReadCSV\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA623C6C-0508-4B11-AD51-FD9907027221}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB1DE48-7B99-4FF3-9820-F6EBF52B6AA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="480" windowWidth="15375" windowHeight="7875" xr2:uid="{88BFBF2D-7389-49F7-AFBC-96501054DF82}"/>
+    <workbookView xWindow="2250" yWindow="480" windowWidth="15375" windowHeight="7875" xr2:uid="{56C2AE74-34BA-498B-8D58-B3F2FC078EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,215 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Joselin</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>Guatemalteca</t>
+  </si>
+  <si>
+    <t>Banca Privada</t>
+  </si>
+  <si>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Cgc</t>
+  </si>
+  <si>
+    <t>Casado</t>
+  </si>
+  <si>
+    <t>Cliente y Empleado</t>
+  </si>
+  <si>
+    <t>Andrade</t>
+  </si>
+  <si>
+    <t>Leslie</t>
+  </si>
+  <si>
+    <t>No definido</t>
+  </si>
+  <si>
+    <t>Citi</t>
+  </si>
+  <si>
+    <t>Divorciado</t>
+  </si>
+  <si>
+    <t>Espinoza</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Cmg</t>
+  </si>
+  <si>
+    <t>Viudo</t>
+  </si>
+  <si>
+    <t>Lainez</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Gcg</t>
+  </si>
+  <si>
+    <t>Unido</t>
+  </si>
+  <si>
+    <t>Estrada</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>MicroFinanzas</t>
+  </si>
+  <si>
+    <t>Escobar</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>No definida</t>
+  </si>
+  <si>
+    <t>No Definido</t>
+  </si>
+  <si>
+    <t>Pineda</t>
+  </si>
+  <si>
+    <t>Gladys</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Danilo</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>Juarez</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>13/02/2017</t>
+  </si>
+  <si>
+    <t>Alravez</t>
+  </si>
+  <si>
+    <t>Edwin</t>
+  </si>
+  <si>
+    <t>14/02/2017</t>
+  </si>
+  <si>
+    <t>Alvizuris</t>
+  </si>
+  <si>
+    <t>Katherin</t>
+  </si>
+  <si>
+    <t>15/02/2017</t>
+  </si>
+  <si>
+    <t>Bercher</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>16/02/2017</t>
+  </si>
+  <si>
+    <t>Way</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>17/02/2017</t>
+  </si>
+  <si>
+    <t>Corado</t>
+  </si>
+  <si>
+    <t>Estuardo</t>
+  </si>
+  <si>
+    <t>18/02/2017</t>
+  </si>
+  <si>
+    <t>Coronado</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>19/02/2017</t>
+  </si>
+  <si>
+    <t>Reyna</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>20/02/2017</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,8 +269,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,13 +585,534 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9095E6-5859-4ED7-92C9-14CAA03CDF04}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D943FC79-2802-4886-BF83-1446107D8DC6}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>42737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1">
+        <v>42827</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1">
+        <v>42888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1">
+        <v>42918</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1">
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="1">
+        <v>43041</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1">
+        <v>43071</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>